<commit_message>
2023-02-27 	PMD, spotbug 수정 버전
</commit_message>
<xml_diff>
--- a/src/main/webapp/_custom/documents/포탈 게시판 DB 설계_v0.1.xlsx
+++ b/src/main/webapp/_custom/documents/포탈 게시판 DB 설계_v0.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace-gcgf\koreg\src\main\webapp\_custom\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD3B1E7-D2F6-4DD6-9C8F-C2AECBDB986B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6F45AD-44A2-4ABC-AE24-CCBEC4EF205A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E060A37E-DECD-4618-86A8-68A94AD9D868}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="371">
   <si>
     <t>게시판</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1258,10 +1258,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>게시물 상단 고정 가능 여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>POPUP_YN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1459,6 +1455,42 @@
   </si>
   <si>
     <t>PT_BOARD_POST_TAG_MAPPING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시물 분류 가능 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시물 TAG 가능 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST_TAG_YN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST_TYPE_YN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시물 분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST_TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시물 고정 가능 여부</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1651,7 +1683,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>639536</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1668,7 +1700,7 @@
       <xdr:grpSpPr>
         <a:xfrm flipH="1">
           <a:off x="285750" y="706771"/>
-          <a:ext cx="353786" cy="4711273"/>
+          <a:ext cx="353786" cy="5137097"/>
           <a:chOff x="7037614" y="476250"/>
           <a:chExt cx="1126672" cy="3701143"/>
         </a:xfrm>
@@ -1791,13 +1823,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>87085</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>81643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>585106</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>95252</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1813,8 +1845,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13041085" y="5191525"/>
-          <a:ext cx="498021" cy="4058933"/>
+          <a:off x="13041085" y="5617349"/>
+          <a:ext cx="498021" cy="4271844"/>
           <a:chOff x="7190014" y="628650"/>
           <a:chExt cx="1126672" cy="3701143"/>
         </a:xfrm>
@@ -1937,13 +1969,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>258536</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>97971</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>606878</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1959,7 +1991,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm flipH="1">
-          <a:off x="258536" y="9040265"/>
+          <a:off x="258536" y="9679000"/>
           <a:ext cx="348342" cy="423103"/>
           <a:chOff x="7085972" y="7322317"/>
           <a:chExt cx="413658" cy="422241"/>
@@ -2080,13 +2112,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>81643</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>81643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>462643</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>84367</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2102,8 +2134,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13035643" y="5191525"/>
-          <a:ext cx="17469971" cy="4048048"/>
+          <a:off x="13035643" y="5617349"/>
+          <a:ext cx="17469971" cy="4260959"/>
           <a:chOff x="7048500" y="4152901"/>
           <a:chExt cx="8096250" cy="3075216"/>
         </a:xfrm>
@@ -2226,13 +2258,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>76199</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>97972</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>574220</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>108857</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2248,8 +2280,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="39408846" y="9466090"/>
-          <a:ext cx="498021" cy="2140002"/>
+          <a:off x="39408846" y="10104825"/>
+          <a:ext cx="498021" cy="2140003"/>
           <a:chOff x="7190014" y="628650"/>
           <a:chExt cx="1126672" cy="3701143"/>
         </a:xfrm>
@@ -2372,13 +2404,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>70756</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>84363</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>285749</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>108856</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2394,8 +2426,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13024756" y="5194245"/>
-          <a:ext cx="29551993" cy="4069817"/>
+          <a:off x="13024756" y="5620069"/>
+          <a:ext cx="29551993" cy="4282728"/>
           <a:chOff x="7949293" y="4370613"/>
           <a:chExt cx="15767957" cy="3290207"/>
         </a:xfrm>
@@ -2518,13 +2550,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>42059</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>192975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>450272</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>11189</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2540,7 +2572,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="725618" y="9135269"/>
+          <a:off x="725618" y="9774004"/>
           <a:ext cx="29767625" cy="2798979"/>
           <a:chOff x="1774844" y="7022468"/>
           <a:chExt cx="12662335" cy="2543353"/>
@@ -2734,13 +2766,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>81644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>536120</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>111580</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2756,7 +2788,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="28557070" y="13707997"/>
+          <a:off x="28557070" y="14346732"/>
           <a:ext cx="498021" cy="3010701"/>
           <a:chOff x="7190014" y="628650"/>
           <a:chExt cx="1126672" cy="3701143"/>
@@ -2880,9 +2912,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2920,7 +2952,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3026,7 +3058,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3168,7 +3200,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3759,7 +3791,7 @@
         <v>141</v>
       </c>
       <c r="F45" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.3">
@@ -3835,14 +3867,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CA19AA-FF60-424C-8C7D-4F9987A47187}">
-  <dimension ref="A1:AB89"/>
+  <dimension ref="A1:AB92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="9" style="3"/>
     <col min="3" max="3" width="26.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="25.125" customWidth="1"/>
@@ -3871,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $D$3, " IS '", C3, "';")</f>
@@ -3882,7 +3915,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -3898,7 +3931,7 @@
         <v>296</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G21" si="0">CONCATENATE(", ", D4, " ", E4, " ", F4)</f>
+        <f t="shared" ref="G4:G23" si="0">CONCATENATE(", ", D4, " ", E4, " ", F4)</f>
         <v>, BRD_ID INTEGER NOT NULL</v>
       </c>
       <c r="H4" t="str">
@@ -3927,7 +3960,7 @@
         <v>, BRD_NM VARCHAR2(255) NOT NULL</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" ref="H5:H21" si="1">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$3, ".", D5, " IS '", C5, "';")</f>
+        <f t="shared" ref="H5:H23" si="1">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$3, ".", D5, " IS '", C5, "';")</f>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.BRD_NM IS '게시판 이름';</v>
       </c>
       <c r="I5" t="s">
@@ -3958,10 +3991,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
+        <v>337</v>
+      </c>
+      <c r="D7" t="s">
         <v>338</v>
-      </c>
-      <c r="D7" t="s">
-        <v>339</v>
       </c>
       <c r="E7" t="s">
         <v>293</v>
@@ -4004,6 +4037,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>368</v>
+      </c>
       <c r="C9" t="s">
         <v>290</v>
       </c>
@@ -4048,11 +4084,14 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>368</v>
+      </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>362</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>365</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -4062,11 +4101,11 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>, POST_FILE_YN VARCHAR2(1) NOT NULL</v>
+        <v>, POST_TYPE_YN VARCHAR2(1) NOT NULL</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_FILE_YN IS '게시물 파일 첨부 여부';</v>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_TYPE_YN IS '게시물 분류 가능 여부';</v>
       </c>
       <c r="I11" t="s">
         <v>300</v>
@@ -4074,10 +4113,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>25</v>
+        <v>363</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>364</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
@@ -4086,346 +4125,361 @@
         <v>296</v>
       </c>
       <c r="G12" t="str">
+        <f t="shared" ref="G12" si="4">CONCATENATE(", ", D12, " ", E12, " ", F12)</f>
+        <v>, POST_TAG_YN VARCHAR2(1) NOT NULL</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" ref="H12" si="5">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$3, ".", D12, " IS '", C12, "';")</f>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_TAG_YN IS '게시물 TAG 가능 여부';</v>
+      </c>
+      <c r="I12" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>296</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>, POST_FILE_YN VARCHAR2(1) NOT NULL</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_FILE_YN IS '게시물 파일 첨부 여부';</v>
+      </c>
+      <c r="I13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>296</v>
+      </c>
+      <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>, POST_CMNT_YN VARCHAR2(1) NOT NULL</v>
       </c>
-      <c r="H12" t="str">
+      <c r="H14" t="str">
         <f t="shared" si="1"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_CMNT_YN IS '게시물 댓글 가능 여부';</v>
       </c>
-      <c r="I12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+      <c r="I14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>98</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" t="s">
         <v>40</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>296</v>
       </c>
-      <c r="G13" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>, POST_CMNT_FILE_YN VARCHAR2(1) NOT NULL</v>
       </c>
-      <c r="H13" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="1"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_CMNT_FILE_YN IS '게시물 댓글 파일 첨부 여부';</v>
       </c>
-      <c r="I13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+      <c r="I15" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C16" t="s">
         <v>306</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E16" t="s">
         <v>40</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>296</v>
       </c>
-      <c r="G14" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>, POST_POPUP_YN VARCHAR2(1) NOT NULL</v>
       </c>
-      <c r="H14" t="str">
+      <c r="H16" t="str">
         <f t="shared" si="1"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_POPUP_YN IS '게시물 팝업 가능 여부';</v>
       </c>
-      <c r="I14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+      <c r="I16" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
         <v>307</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>45</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F17" t="s">
         <v>296</v>
       </c>
-      <c r="G15" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>, POST_SECRET_YN VARCHAR2(1) NOT NULL</v>
       </c>
-      <c r="H15" t="str">
+      <c r="H17" t="str">
         <f t="shared" si="1"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_SECRET_YN IS '게시물 비밀 가능 여부';</v>
       </c>
-      <c r="I15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>312</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="I17" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C18" t="s">
+        <v>370</v>
+      </c>
+      <c r="D18" t="s">
         <v>46</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
         <v>40</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F18" t="s">
         <v>296</v>
       </c>
-      <c r="G16" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>, POST_FIX_YN VARCHAR2(1) NOT NULL</v>
       </c>
-      <c r="H16" t="str">
+      <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_FIX_YN IS '게시물 상단 고정 가능 여부';</v>
-      </c>
-      <c r="I16" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD.POST_FIX_YN IS '게시물 고정 가능 여부';</v>
+      </c>
+      <c r="I18" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="D17" t="s">
-        <v>318</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D19" t="s">
+        <v>317</v>
+      </c>
+      <c r="E19" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F19" t="s">
         <v>296</v>
       </c>
-      <c r="G17" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="0"/>
         <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
       </c>
-      <c r="H17" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="1"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.DEL_YN IS '삭제 여부';</v>
       </c>
-      <c r="I17" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+      <c r="I19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>289</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>43</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F20" t="s">
         <v>296</v>
       </c>
-      <c r="G18" t="str">
+      <c r="G20" t="str">
         <f t="shared" si="0"/>
         <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
       </c>
-      <c r="H18" t="str">
+      <c r="H20" t="str">
         <f t="shared" si="1"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.CRT_DT_TM IS '생성 일시';</v>
       </c>
-      <c r="I18" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+      <c r="I20" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>305</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" t="s">
         <v>41</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>296</v>
       </c>
-      <c r="G19" t="str">
+      <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
       </c>
-      <c r="H19" t="str">
+      <c r="H21" t="str">
         <f t="shared" si="1"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.CRT_USR_ID IS '생성자 ID';</v>
       </c>
-      <c r="I19" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="I21" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>302</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E22" t="s">
         <v>43</v>
       </c>
-      <c r="G20" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
       </c>
-      <c r="H20" t="str">
+      <c r="H22" t="str">
         <f t="shared" si="1"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.MOD_DT_TM IS '수정 일시';</v>
       </c>
-      <c r="I20" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+      <c r="I22" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
         <v>7</v>
       </c>
-      <c r="D21" t="s">
-        <v>337</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D23" t="s">
+        <v>336</v>
+      </c>
+      <c r="E23" t="s">
         <v>41</v>
       </c>
-      <c r="G21" t="str">
+      <c r="G23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">, MOD_USR_ID VARCHAR2(20) </v>
       </c>
-      <c r="H21" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="1"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD.MOD_USR_ID IS '수정자 ID';</v>
       </c>
-      <c r="I21" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="1" t="s">
+      <c r="I23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D24" t="s">
-        <v>353</v>
-      </c>
-      <c r="H24" t="str">
-        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $D$24, " IS '", C24, "';")</f>
+      <c r="D26" t="s">
+        <v>352</v>
+      </c>
+      <c r="H26" t="str">
+        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $D$26, " IS '", C26, "';")</f>
         <v>COMMENT ON TABLE PORTAL.PT_BOARD_POST IS '게시물';</v>
       </c>
-      <c r="I24" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="I26" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="G25" t="str">
-        <f>CONCATENATE(", ", D25, " ", E25, " ", F25)</f>
+      <c r="G27" t="str">
+        <f>CONCATENATE(", ", D27, " ", E27, " ", F27)</f>
         <v>, POST_ID INTEGER NOT NULL</v>
       </c>
-      <c r="H25" t="str">
-        <f t="shared" ref="H25:H39" si="4">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$24, ".", D25, " IS '", C25, "';")</f>
+      <c r="H27" t="str">
+        <f t="shared" ref="H27:H42" si="6">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$26, ".", D27, " IS '", C27, "';")</f>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POST_ID IS '게시물 ID';</v>
       </c>
-      <c r="I25" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="I27" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="G26" t="str">
-        <f t="shared" ref="G26:G39" si="5">CONCATENATE(", ", D26, " ", E26, " ", F26)</f>
+      <c r="G28" t="str">
+        <f t="shared" ref="G28:G42" si="7">CONCATENATE(", ", D28, " ", E28, " ", F28)</f>
         <v>, BRD_ID INTEGER NOT NULL</v>
       </c>
-      <c r="H26" t="str">
-        <f t="shared" si="4"/>
+      <c r="H28" t="str">
+        <f t="shared" si="6"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.BRD_ID IS '게시판 ID';</v>
-      </c>
-      <c r="I26" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>303</v>
-      </c>
-      <c r="D27" t="s">
-        <v>304</v>
-      </c>
-      <c r="E27" t="s">
-        <v>293</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">, POST_TITLE VARCHAR2(255) </v>
-      </c>
-      <c r="H27" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POST_TITLE IS '게시물 제목';</v>
-      </c>
-      <c r="I27" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">, POST_CONTENT CLOB </v>
-      </c>
-      <c r="H28" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POST_CONTENT IS '게시물 내용';</v>
       </c>
       <c r="I28" t="s">
         <v>300</v>
@@ -4433,21 +4487,21 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>27</v>
+        <v>366</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>367</v>
       </c>
       <c r="E29" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">, POST_VIEW_AUTH VARCHAR2(2000) </v>
+        <f t="shared" ref="G29" si="8">CONCATENATE(", ", D29, " ", E29, " ", F29)</f>
+        <v xml:space="preserve">, POST_TYPE VARCHAR2(255) </v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POST_VIEW_AUTH IS '게시물 보기 권한';</v>
+        <f t="shared" ref="H29" si="9">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$26, ".", D29, " IS '", C29, "';")</f>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POST_TYPE IS '게시물 분류';</v>
       </c>
       <c r="I29" t="s">
         <v>300</v>
@@ -4455,21 +4509,21 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>8</v>
+        <v>303</v>
       </c>
       <c r="D30" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
+        <v>293</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">, POPUP_YN VARCHAR2(1) </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">, POST_TITLE VARCHAR2(255) </v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POPUP_YN IS '팝업 가능 여부';</v>
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POST_TITLE IS '게시물 제목';</v>
       </c>
       <c r="I30" t="s">
         <v>300</v>
@@ -4477,21 +4531,21 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>316</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>314</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">, POPUP_START_DT_TM TIMESTAMP </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">, POST_CONTENT CLOB </v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POPUP_START_DT_TM IS '팝업 시작 일자';</v>
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POST_CONTENT IS '게시물 내용';</v>
       </c>
       <c r="I31" t="s">
         <v>300</v>
@@ -4499,21 +4553,21 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>317</v>
+        <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>315</v>
+        <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>301</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">, POPUP_END_DT_TM TIMESTAMP </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">, POST_VIEW_AUTH VARCHAR2(2000) </v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POPUP_END_DT_TM IS '팝업 종료 일자';</v>
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POST_VIEW_AUTH IS '게시물 보기 권한';</v>
       </c>
       <c r="I32" t="s">
         <v>300</v>
@@ -4521,21 +4575,21 @@
     </row>
     <row r="33" spans="2:26" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>308</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E33" t="s">
         <v>40</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">, SECRET_YN VARCHAR2(1) </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">, POPUP_YN VARCHAR2(1) </v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.SECRET_YN IS '비밀 가능 여부';</v>
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POPUP_YN IS '팝업 가능 여부';</v>
       </c>
       <c r="I33" t="s">
         <v>300</v>
@@ -4543,21 +4597,21 @@
     </row>
     <row r="34" spans="2:26" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="D34" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E34" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">, FIX_YN VARCHAR2(1) </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">, POPUP_START_DT_TM TIMESTAMP </v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.FIX_YN IS '고정 가능 여부';</v>
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POPUP_START_DT_TM IS '팝업 시작 일자';</v>
       </c>
       <c r="I34" t="s">
         <v>300</v>
@@ -4565,24 +4619,21 @@
     </row>
     <row r="35" spans="2:26" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>5</v>
+        <v>316</v>
       </c>
       <c r="D35" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" t="s">
-        <v>296</v>
+        <v>43</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="5"/>
-        <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">, POPUP_END_DT_TM TIMESTAMP </v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.DEL_YN IS '삭제 여부';</v>
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.POPUP_END_DT_TM IS '팝업 종료 일자';</v>
       </c>
       <c r="I35" t="s">
         <v>300</v>
@@ -4590,24 +4641,21 @@
     </row>
     <row r="36" spans="2:26" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>15</v>
+        <v>308</v>
       </c>
       <c r="D36" t="s">
-        <v>289</v>
+        <v>310</v>
       </c>
       <c r="E36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" t="s">
-        <v>296</v>
+        <v>40</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="5"/>
-        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">, SECRET_YN VARCHAR2(1) </v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.CRT_DT_TM IS '생성 일시';</v>
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.SECRET_YN IS '비밀 가능 여부';</v>
       </c>
       <c r="I36" t="s">
         <v>300</v>
@@ -4615,24 +4663,21 @@
     </row>
     <row r="37" spans="2:26" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>6</v>
+        <v>309</v>
       </c>
       <c r="D37" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="E37" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" t="s">
-        <v>296</v>
+        <v>40</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="5"/>
-        <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">, FIX_YN VARCHAR2(1) </v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.CRT_USR_ID IS '생성자 ID';</v>
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.FIX_YN IS '고정 가능 여부';</v>
       </c>
       <c r="I37" t="s">
         <v>300</v>
@@ -4640,21 +4685,24 @@
     </row>
     <row r="38" spans="2:26" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="F38" t="s">
+        <v>296</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
+        <f t="shared" si="7"/>
+        <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="4"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.MOD_DT_TM IS '수정 일시';</v>
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.DEL_YN IS '삭제 여부';</v>
       </c>
       <c r="I38" t="s">
         <v>300</v>
@@ -4662,502 +4710,400 @@
     </row>
     <row r="39" spans="2:26" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>289</v>
+      </c>
+      <c r="E39" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" t="s">
+        <v>296</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="7"/>
+        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.CRT_DT_TM IS '생성 일시';</v>
+      </c>
+      <c r="I39" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>305</v>
+      </c>
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" t="s">
+        <v>296</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="7"/>
+        <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.CRT_USR_ID IS '생성자 ID';</v>
+      </c>
+      <c r="I40" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" t="s">
+        <v>302</v>
+      </c>
+      <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.MOD_DT_TM IS '수정 일시';</v>
+      </c>
+      <c r="I41" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D42" t="s">
         <v>118</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E42" t="s">
         <v>41</v>
       </c>
-      <c r="G39" t="str">
-        <f t="shared" si="5"/>
+      <c r="G42" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">, MOD_USR_ID VARCHAR2(20) </v>
       </c>
-      <c r="H39" t="str">
-        <f t="shared" si="4"/>
+      <c r="H42" t="str">
+        <f t="shared" si="6"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST.MOD_USR_ID IS '수정자 ID';</v>
       </c>
-      <c r="I39" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="42" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C42" s="1" t="s">
+      <c r="I42" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="45" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="C45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D42" t="s">
-        <v>354</v>
-      </c>
-      <c r="H42" t="str">
-        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $D$42, " IS '", C42, "';")</f>
+      <c r="D45" t="s">
+        <v>353</v>
+      </c>
+      <c r="H45" t="str">
+        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $D$45, " IS '", C45, "';")</f>
         <v>COMMENT ON TABLE PORTAL.PT_BOARD_POST_COMMENT IS '댓글';</v>
       </c>
-      <c r="I42" t="s">
-        <v>300</v>
-      </c>
-      <c r="L42" s="1" t="s">
+      <c r="I45" t="s">
+        <v>300</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M42" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q42" t="str">
-        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $M$42, " IS '", L42, "';")</f>
+      <c r="M45" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q45" t="str">
+        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $M$45, " IS '", L45, "';")</f>
         <v>COMMENT ON TABLE PORTAL.PT_BOARD_POST_FILE IS '파일';</v>
       </c>
-      <c r="R42" t="s">
-        <v>300</v>
-      </c>
-      <c r="W42" s="1" t="s">
+      <c r="R45" t="s">
+        <v>300</v>
+      </c>
+      <c r="W45" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="X42" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="43" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+      <c r="X45" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="46" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B46" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E46" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F46" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="G43" t="str">
-        <f>CONCATENATE(", ", D43, " ", E43, " ", F43)</f>
+      <c r="G46" t="str">
+        <f>CONCATENATE(", ", D46, " ", E46, " ", F46)</f>
         <v>, CMNT_ID INTEGER NOT NULL</v>
       </c>
-      <c r="H43" t="str">
-        <f t="shared" ref="H43:H51" si="6">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$42, ".", D43, " IS '", C43, "';")</f>
+      <c r="H46" t="str">
+        <f t="shared" ref="H46:H54" si="10">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$45, ".", D46, " IS '", C46, "';")</f>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.CMNT_ID IS '댓글 ID';</v>
       </c>
-      <c r="I43" t="s">
-        <v>300</v>
-      </c>
-      <c r="K43" t="s">
+      <c r="I46" t="s">
+        <v>300</v>
+      </c>
+      <c r="K46" t="s">
         <v>22</v>
       </c>
-      <c r="L43" s="6" t="s">
+      <c r="L46" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M43" s="6" t="s">
+      <c r="M46" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="N43" s="6" t="s">
+      <c r="N46" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="O43" s="6" t="s">
+      <c r="O46" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="P43" t="str">
-        <f>CONCATENATE(", ", M43, " ", N43, " ", O43)</f>
+      <c r="P46" t="str">
+        <f>CONCATENATE(", ", M46, " ", N46, " ", O46)</f>
         <v>, FILE_ID INTEGER NOT NULL</v>
       </c>
-      <c r="Q43" t="str">
-        <f t="shared" ref="Q43:Q56" si="7">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $M$42, ".", M43, " IS '", L43, "';")</f>
+      <c r="Q46" t="str">
+        <f t="shared" ref="Q46:Q59" si="11">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $M$45, ".", M46, " IS '", L46, "';")</f>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.FILE_ID IS '파일 ID';</v>
       </c>
-      <c r="R43" t="s">
-        <v>300</v>
-      </c>
-      <c r="V43" t="s">
+      <c r="R46" t="s">
+        <v>300</v>
+      </c>
+      <c r="V46" t="s">
         <v>22</v>
       </c>
-      <c r="W43" s="6" t="s">
+      <c r="W46" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="X43" s="6" t="s">
+      <c r="X46" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="Y43" s="6" t="s">
+      <c r="Y46" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="Z43" s="6" t="s">
+      <c r="Z46" s="6" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
+    <row r="47" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="F44" s="6"/>
-      <c r="G44" t="str">
-        <f t="shared" ref="G44:G51" si="8">CONCATENATE(", ", D44, " ", E44, " ", F44)</f>
+      <c r="F47" s="6"/>
+      <c r="G47" t="str">
+        <f t="shared" ref="G47:G54" si="12">CONCATENATE(", ", D47, " ", E47, " ", F47)</f>
         <v xml:space="preserve">, POST_ID INTEGER </v>
       </c>
-      <c r="H44" t="str">
-        <f t="shared" si="6"/>
+      <c r="H47" t="str">
+        <f t="shared" si="10"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.POST_ID IS '게시물 ID';</v>
       </c>
-      <c r="I44" t="s">
-        <v>300</v>
-      </c>
-      <c r="K44" t="s">
+      <c r="I47" t="s">
+        <v>300</v>
+      </c>
+      <c r="K47" t="s">
         <v>23</v>
       </c>
-      <c r="L44" s="6" t="s">
+      <c r="L47" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M44" s="6" t="s">
+      <c r="M47" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="N44" s="6" t="s">
+      <c r="N47" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="O44" s="6"/>
-      <c r="P44" t="str">
-        <f t="shared" ref="P44:P56" si="9">CONCATENATE(", ", M44, " ", N44, " ", O44)</f>
+      <c r="O47" s="6"/>
+      <c r="P47" t="str">
+        <f t="shared" ref="P47:P59" si="13">CONCATENATE(", ", M47, " ", N47, " ", O47)</f>
         <v xml:space="preserve">, POST_ID INTEGER </v>
       </c>
-      <c r="Q44" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q47" t="str">
+        <f t="shared" si="11"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.POST_ID IS '게시물 ID';</v>
       </c>
-      <c r="R44" t="s">
-        <v>300</v>
-      </c>
-      <c r="V44" t="s">
+      <c r="R47" t="s">
+        <v>300</v>
+      </c>
+      <c r="V47" t="s">
         <v>23</v>
       </c>
-      <c r="W44" t="s">
+      <c r="W47" t="s">
         <v>4</v>
       </c>
-      <c r="X44" t="s">
+      <c r="X47" t="s">
         <v>29</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="Y47" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="45" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
+    <row r="48" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B48" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C48" t="s">
         <v>38</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D48" t="s">
         <v>119</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E48" t="s">
         <v>295</v>
       </c>
-      <c r="G45" t="str">
-        <f t="shared" si="8"/>
+      <c r="G48" t="str">
+        <f t="shared" si="12"/>
         <v xml:space="preserve">, PARENT_CMNT_ID INTEGER </v>
       </c>
-      <c r="H45" t="str">
-        <f t="shared" si="6"/>
+      <c r="H48" t="str">
+        <f t="shared" si="10"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.PARENT_CMNT_ID IS '상위 댓글 ID';</v>
       </c>
-      <c r="I45" t="s">
-        <v>300</v>
-      </c>
-      <c r="K45" t="s">
+      <c r="I48" t="s">
+        <v>300</v>
+      </c>
+      <c r="K48" t="s">
         <v>23</v>
       </c>
-      <c r="L45" t="s">
+      <c r="L48" t="s">
         <v>298</v>
       </c>
-      <c r="M45" t="s">
+      <c r="M48" t="s">
         <v>297</v>
       </c>
-      <c r="N45" t="s">
+      <c r="N48" t="s">
         <v>68</v>
       </c>
-      <c r="P45" t="str">
-        <f t="shared" si="9"/>
+      <c r="P48" t="str">
+        <f t="shared" si="13"/>
         <v xml:space="preserve">, FILE_TYPE VARCHAR2(100) </v>
       </c>
-      <c r="Q45" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q48" t="str">
+        <f t="shared" si="11"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.FILE_TYPE IS '파일 분류';</v>
       </c>
-      <c r="R45" t="s">
-        <v>300</v>
-      </c>
-      <c r="W45" t="s">
+      <c r="R48" t="s">
+        <v>300</v>
+      </c>
+      <c r="W48" t="s">
         <v>49</v>
       </c>
-      <c r="X45" t="s">
+      <c r="X48" t="s">
         <v>52</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="Y48" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="46" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
+    <row r="49" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
         <v>19</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D49" t="s">
         <v>154</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E49" t="s">
         <v>42</v>
       </c>
-      <c r="G46" t="str">
-        <f t="shared" si="8"/>
+      <c r="G49" t="str">
+        <f t="shared" si="12"/>
         <v xml:space="preserve">, CMNT_CONTENT CLOB </v>
       </c>
-      <c r="H46" t="str">
-        <f t="shared" si="6"/>
+      <c r="H49" t="str">
+        <f t="shared" si="10"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.CMNT_CONTENT IS '댓글 내용';</v>
       </c>
-      <c r="I46" t="s">
-        <v>300</v>
-      </c>
-      <c r="L46" t="s">
+      <c r="I49" t="s">
+        <v>300</v>
+      </c>
+      <c r="L49" t="s">
         <v>38</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M49" t="s">
         <v>89</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N49" t="s">
         <v>295</v>
       </c>
-      <c r="P46" t="str">
-        <f t="shared" si="9"/>
+      <c r="P49" t="str">
+        <f t="shared" si="13"/>
         <v xml:space="preserve">, PARENT_CMNT_ID INTEGER </v>
       </c>
-      <c r="Q46" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q49" t="str">
+        <f t="shared" si="11"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.PARENT_CMNT_ID IS '상위 댓글 ID';</v>
       </c>
-      <c r="R46" t="s">
-        <v>300</v>
-      </c>
-      <c r="W46" t="s">
+      <c r="R49" t="s">
+        <v>300</v>
+      </c>
+      <c r="W49" t="s">
         <v>5</v>
       </c>
-      <c r="X46" t="s">
+      <c r="X49" t="s">
         <v>113</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="Y49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
+    <row r="50" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
         <v>5</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D50" t="s">
         <v>113</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E50" t="s">
         <v>40</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F50" t="s">
         <v>296</v>
       </c>
-      <c r="G47" t="str">
-        <f t="shared" si="8"/>
+      <c r="G50" t="str">
+        <f t="shared" si="12"/>
         <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
       </c>
-      <c r="H47" t="str">
-        <f t="shared" si="6"/>
+      <c r="H50" t="str">
+        <f t="shared" si="10"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.DEL_YN IS '삭제 여부';</v>
       </c>
-      <c r="I47" t="s">
-        <v>300</v>
-      </c>
-      <c r="L47" t="s">
+      <c r="I50" t="s">
+        <v>300</v>
+      </c>
+      <c r="L50" t="s">
         <v>11</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M50" t="s">
         <v>124</v>
-      </c>
-      <c r="N47" t="s">
-        <v>39</v>
-      </c>
-      <c r="O47" t="s">
-        <v>296</v>
-      </c>
-      <c r="P47" t="str">
-        <f t="shared" si="9"/>
-        <v>, SRV_FILE_PATH VARCHAR2(255) NOT NULL</v>
-      </c>
-      <c r="Q47" t="str">
-        <f t="shared" si="7"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.SRV_FILE_PATH IS '서버 파일 경로';</v>
-      </c>
-      <c r="R47" t="s">
-        <v>300</v>
-      </c>
-      <c r="W47" t="s">
-        <v>15</v>
-      </c>
-      <c r="X47" t="s">
-        <v>289</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z47" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="48" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" t="s">
-        <v>76</v>
-      </c>
-      <c r="E48" t="s">
-        <v>43</v>
-      </c>
-      <c r="F48" t="s">
-        <v>296</v>
-      </c>
-      <c r="G48" t="str">
-        <f t="shared" si="8"/>
-        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
-      </c>
-      <c r="H48" t="str">
-        <f t="shared" si="6"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.CRT_DT_TM IS '생성 일시';</v>
-      </c>
-      <c r="I48" t="s">
-        <v>300</v>
-      </c>
-      <c r="L48" t="s">
-        <v>12</v>
-      </c>
-      <c r="M48" t="s">
-        <v>125</v>
-      </c>
-      <c r="N48" t="s">
-        <v>39</v>
-      </c>
-      <c r="O48" t="s">
-        <v>296</v>
-      </c>
-      <c r="P48" t="str">
-        <f t="shared" si="9"/>
-        <v>, SRV_FILE_NM VARCHAR2(255) NOT NULL</v>
-      </c>
-      <c r="Q48" t="str">
-        <f t="shared" si="7"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.SRV_FILE_NM IS '서버 파일 명';</v>
-      </c>
-      <c r="R48" t="s">
-        <v>300</v>
-      </c>
-      <c r="W48" t="s">
-        <v>6</v>
-      </c>
-      <c r="X48" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y48" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z48" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="49" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" t="s">
-        <v>75</v>
-      </c>
-      <c r="E49" t="s">
-        <v>41</v>
-      </c>
-      <c r="F49" t="s">
-        <v>296</v>
-      </c>
-      <c r="G49" t="str">
-        <f t="shared" si="8"/>
-        <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
-      </c>
-      <c r="H49" t="str">
-        <f t="shared" si="6"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.CRT_USR_ID IS '생성자 ID';</v>
-      </c>
-      <c r="I49" t="s">
-        <v>300</v>
-      </c>
-      <c r="L49" t="s">
-        <v>13</v>
-      </c>
-      <c r="M49" t="s">
-        <v>120</v>
-      </c>
-      <c r="N49" t="s">
-        <v>39</v>
-      </c>
-      <c r="O49" t="s">
-        <v>296</v>
-      </c>
-      <c r="P49" t="str">
-        <f t="shared" si="9"/>
-        <v>, ORG_FILE_NM VARCHAR2(255) NOT NULL</v>
-      </c>
-      <c r="Q49" t="str">
-        <f t="shared" si="7"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.ORG_FILE_NM IS '원본 파일 명';</v>
-      </c>
-      <c r="R49" t="s">
-        <v>300</v>
-      </c>
-      <c r="W49" t="s">
-        <v>16</v>
-      </c>
-      <c r="X49" t="s">
-        <v>302</v>
-      </c>
-      <c r="Y49" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" t="s">
-        <v>302</v>
-      </c>
-      <c r="E50" t="s">
-        <v>43</v>
-      </c>
-      <c r="G50" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
-      </c>
-      <c r="H50" t="str">
-        <f t="shared" si="6"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.MOD_DT_TM IS '수정 일시';</v>
-      </c>
-      <c r="I50" t="s">
-        <v>300</v>
-      </c>
-      <c r="L50" t="s">
-        <v>57</v>
-      </c>
-      <c r="M50" t="s">
-        <v>129</v>
       </c>
       <c r="N50" t="s">
         <v>39</v>
@@ -5166,1380 +5112,1554 @@
         <v>296</v>
       </c>
       <c r="P50" t="str">
-        <f t="shared" si="9"/>
-        <v>, FILE_EXT VARCHAR2(255) NOT NULL</v>
+        <f t="shared" si="13"/>
+        <v>, SRV_FILE_PATH VARCHAR2(255) NOT NULL</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" si="7"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.FILE_EXT IS '파일 확장자';</v>
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.SRV_FILE_PATH IS '서버 파일 경로';</v>
       </c>
       <c r="R50" t="s">
         <v>300</v>
       </c>
       <c r="W50" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="X50" t="s">
-        <v>118</v>
+        <v>289</v>
       </c>
       <c r="Y50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="3:28" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="51" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="E51" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="F51" t="s">
+        <v>296</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">, MOD_USR_ID VARCHAR2(20) </v>
+        <f t="shared" si="12"/>
+        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="6"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.MOD_USR_ID IS '수정자 ID';</v>
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.CRT_DT_TM IS '생성 일시';</v>
       </c>
       <c r="I51" t="s">
         <v>300</v>
       </c>
       <c r="L51" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M51" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="N51" t="s">
-        <v>295</v>
+        <v>39</v>
       </c>
       <c r="O51" t="s">
         <v>296</v>
       </c>
       <c r="P51" t="str">
-        <f t="shared" si="9"/>
-        <v>, FILE_SIZE INTEGER NOT NULL</v>
+        <f t="shared" si="13"/>
+        <v>, SRV_FILE_NM VARCHAR2(255) NOT NULL</v>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" si="7"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.FILE_SIZE IS '파일 사이즈';</v>
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.SRV_FILE_NM IS '서버 파일 명';</v>
       </c>
       <c r="R51" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="52" spans="3:28" x14ac:dyDescent="0.3">
+      <c r="W51" t="s">
+        <v>6</v>
+      </c>
+      <c r="X51" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="52" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" t="s">
+        <v>296</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="12"/>
+        <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.CRT_USR_ID IS '생성자 ID';</v>
+      </c>
+      <c r="I52" t="s">
+        <v>300</v>
+      </c>
       <c r="L52" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="M52" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="N52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O52" t="s">
         <v>296</v>
       </c>
       <c r="P52" t="str">
-        <f t="shared" si="9"/>
-        <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
+        <f t="shared" si="13"/>
+        <v>, ORG_FILE_NM VARCHAR2(255) NOT NULL</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" si="7"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.DEL_YN IS '삭제 여부';</v>
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.ORG_FILE_NM IS '원본 파일 명';</v>
       </c>
       <c r="R52" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="53" spans="3:28" x14ac:dyDescent="0.3">
+      <c r="W52" t="s">
+        <v>16</v>
+      </c>
+      <c r="X52" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>302</v>
+      </c>
+      <c r="E53" t="s">
+        <v>43</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.MOD_DT_TM IS '수정 일시';</v>
+      </c>
+      <c r="I53" t="s">
+        <v>300</v>
+      </c>
       <c r="L53" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="M53" t="s">
-        <v>289</v>
+        <v>129</v>
       </c>
       <c r="N53" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="O53" t="s">
         <v>296</v>
       </c>
       <c r="P53" t="str">
-        <f t="shared" si="9"/>
-        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
+        <f t="shared" si="13"/>
+        <v>, FILE_EXT VARCHAR2(255) NOT NULL</v>
       </c>
       <c r="Q53" t="str">
-        <f t="shared" si="7"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.CRT_DT_TM IS '생성 일시';</v>
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.FILE_EXT IS '파일 확장자';</v>
       </c>
       <c r="R53" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="54" spans="3:28" x14ac:dyDescent="0.3">
+      <c r="W53" t="s">
+        <v>7</v>
+      </c>
+      <c r="X53" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" t="s">
+        <v>41</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">, MOD_USR_ID VARCHAR2(20) </v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_COMMENT.MOD_USR_ID IS '수정자 ID';</v>
+      </c>
+      <c r="I54" t="s">
+        <v>300</v>
+      </c>
       <c r="L54" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="M54" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="N54" t="s">
-        <v>41</v>
+        <v>295</v>
       </c>
       <c r="O54" t="s">
         <v>296</v>
       </c>
       <c r="P54" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
+        <v>, FILE_SIZE INTEGER NOT NULL</v>
+      </c>
+      <c r="Q54" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.FILE_SIZE IS '파일 사이즈';</v>
+      </c>
+      <c r="R54" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="55" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="L55" t="s">
+        <v>5</v>
+      </c>
+      <c r="M55" t="s">
+        <v>113</v>
+      </c>
+      <c r="N55" t="s">
+        <v>40</v>
+      </c>
+      <c r="O55" t="s">
+        <v>296</v>
+      </c>
+      <c r="P55" t="str">
+        <f t="shared" si="13"/>
+        <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
+      </c>
+      <c r="Q55" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.DEL_YN IS '삭제 여부';</v>
+      </c>
+      <c r="R55" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="L56" t="s">
+        <v>15</v>
+      </c>
+      <c r="M56" t="s">
+        <v>289</v>
+      </c>
+      <c r="N56" t="s">
+        <v>43</v>
+      </c>
+      <c r="O56" t="s">
+        <v>296</v>
+      </c>
+      <c r="P56" t="str">
+        <f t="shared" si="13"/>
+        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
+      </c>
+      <c r="Q56" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.CRT_DT_TM IS '생성 일시';</v>
+      </c>
+      <c r="R56" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="57" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="L57" t="s">
+        <v>6</v>
+      </c>
+      <c r="M57" t="s">
+        <v>75</v>
+      </c>
+      <c r="N57" t="s">
+        <v>41</v>
+      </c>
+      <c r="O57" t="s">
+        <v>296</v>
+      </c>
+      <c r="P57" t="str">
+        <f t="shared" si="13"/>
         <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
       </c>
-      <c r="Q54" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q57" t="str">
+        <f t="shared" si="11"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.CRT_USR_ID IS '생성자 ID';</v>
       </c>
-      <c r="R54" t="s">
-        <v>300</v>
-      </c>
-      <c r="W54" s="1" t="s">
+      <c r="R57" t="s">
+        <v>300</v>
+      </c>
+      <c r="W57" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="X54" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="55" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="L55" t="s">
+      <c r="X57" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="58" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="L58" t="s">
         <v>16</v>
       </c>
-      <c r="M55" t="s">
+      <c r="M58" t="s">
         <v>302</v>
       </c>
-      <c r="N55" t="s">
+      <c r="N58" t="s">
         <v>43</v>
       </c>
-      <c r="P55" t="str">
-        <f t="shared" si="9"/>
+      <c r="P58" t="str">
+        <f t="shared" si="13"/>
         <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
       </c>
-      <c r="Q55" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q58" t="str">
+        <f t="shared" si="11"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.MOD_DT_TM IS '수정 일시';</v>
       </c>
-      <c r="R55" t="s">
-        <v>300</v>
-      </c>
-      <c r="V55" t="s">
+      <c r="R58" t="s">
+        <v>300</v>
+      </c>
+      <c r="V58" t="s">
         <v>22</v>
       </c>
-      <c r="W55" s="6" t="s">
+      <c r="W58" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="X55" s="6" t="s">
+      <c r="X58" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="Y55" s="6" t="s">
+      <c r="Y58" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="Z55" s="6" t="s">
+      <c r="Z58" s="6" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="56" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="L56" t="s">
+    <row r="59" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="L59" t="s">
         <v>7</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M59" t="s">
         <v>118</v>
       </c>
-      <c r="N56" t="s">
+      <c r="N59" t="s">
         <v>41</v>
       </c>
-      <c r="P56" t="str">
-        <f t="shared" si="9"/>
+      <c r="P59" t="str">
+        <f t="shared" si="13"/>
         <v xml:space="preserve">, MOD_USR_ID VARCHAR2(20) </v>
       </c>
-      <c r="Q56" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q59" t="str">
+        <f t="shared" si="11"/>
         <v>COMMENT ON COLUMN PORTAL.PT_BOARD_POST_FILE.MOD_USR_ID IS '수정자 ID';</v>
       </c>
-      <c r="R56" t="s">
-        <v>300</v>
-      </c>
-      <c r="W56" t="s">
+      <c r="R59" t="s">
+        <v>300</v>
+      </c>
+      <c r="W59" t="s">
         <v>50</v>
       </c>
-      <c r="X56" t="s">
+      <c r="X59" t="s">
         <v>86</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Y59" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="W57" t="s">
+    <row r="60" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="W60" t="s">
         <v>15</v>
       </c>
-      <c r="X57" t="s">
+      <c r="X60" t="s">
         <v>289</v>
       </c>
-      <c r="Y57" t="s">
+      <c r="Y60" t="s">
         <v>43</v>
       </c>
-      <c r="Z57" t="s">
+      <c r="Z60" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="58" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="W58" t="s">
+    <row r="61" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="W61" t="s">
         <v>6</v>
       </c>
-      <c r="X58" t="s">
+      <c r="X61" t="s">
         <v>75</v>
       </c>
-      <c r="Y58" t="s">
+      <c r="Y61" t="s">
         <v>41</v>
       </c>
-      <c r="Z58" t="s">
+      <c r="Z61" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="59" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="W59" t="s">
+    <row r="62" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="W62" t="s">
         <v>16</v>
       </c>
-      <c r="X59" t="s">
+      <c r="X62" t="s">
         <v>302</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="Y62" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="W60" t="s">
+    <row r="63" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="W63" t="s">
         <v>7</v>
       </c>
-      <c r="X60" t="s">
+      <c r="X63" t="s">
         <v>118</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="Y63" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C64" s="1" t="s">
+    <row r="67" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C67" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D64" t="s">
-        <v>355</v>
-      </c>
-      <c r="H64" t="str">
-        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $D$64, " IS '", C64, "';")</f>
+      <c r="D67" t="s">
+        <v>354</v>
+      </c>
+      <c r="H67" t="str">
+        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $D$67, " IS '", C67, "';")</f>
         <v>COMMENT ON TABLE PORTAL.PT_PORTAL_LOG IS '포탈 로그';</v>
       </c>
-      <c r="I64" t="s">
-        <v>300</v>
-      </c>
-      <c r="L64" s="1" t="s">
+      <c r="I67" t="s">
+        <v>300</v>
+      </c>
+      <c r="L67" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="M64" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q64" t="str">
-        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $M$64, " IS '", L64, "';")</f>
+      <c r="M67" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q67" t="str">
+        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $M$67, " IS '", L67, "';")</f>
         <v>COMMENT ON TABLE PORTAL.PT_PORTAL_CODE_TYPE IS '포탈 코드 분류 테이블';</v>
       </c>
-      <c r="R64" t="s">
-        <v>300</v>
-      </c>
-      <c r="W64" s="1" t="s">
+      <c r="R67" t="s">
+        <v>300</v>
+      </c>
+      <c r="W67" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="X64" t="s">
-        <v>360</v>
-      </c>
-      <c r="AB64" t="str">
-        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $X$64, " IS '", W64, "';")</f>
+      <c r="X67" t="s">
+        <v>359</v>
+      </c>
+      <c r="AB67" t="str">
+        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $X$67, " IS '", W67, "';")</f>
         <v>COMMENT ON TABLE PORTAL.PT_PORTAL_ADMIN IS '포탈 관리자';</v>
       </c>
     </row>
-    <row r="65" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
+    <row r="68" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B68" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C68" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D68" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E68" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="F65" s="6" t="s">
+      <c r="F68" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="G65" t="str">
-        <f>CONCATENATE(", ", D65, " ", E65, " ", F65)</f>
+      <c r="G68" t="str">
+        <f>CONCATENATE(", ", D68, " ", E68, " ", F68)</f>
         <v>, LOG_ID INTEGER NOT NULL</v>
       </c>
-      <c r="H65" t="str">
-        <f t="shared" ref="H65:H77" si="10">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$64, ".", D65, " IS '", C65, "';")</f>
+      <c r="H68" t="str">
+        <f t="shared" ref="H68:H80" si="14">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $D$67, ".", D68, " IS '", C68, "';")</f>
         <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.LOG_ID IS '로그 ID';</v>
       </c>
-      <c r="I65" t="s">
-        <v>300</v>
-      </c>
-      <c r="K65" t="s">
+      <c r="I68" t="s">
+        <v>300</v>
+      </c>
+      <c r="K68" t="s">
         <v>22</v>
       </c>
-      <c r="L65" s="6" t="s">
+      <c r="L68" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="M65" s="6" t="s">
+      <c r="M68" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="N65" s="6" t="s">
+      <c r="N68" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="O65" s="6" t="s">
+      <c r="O68" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="P65" t="str">
-        <f>CONCATENATE(", ", M65, " ", N65, " ", O65)</f>
+      <c r="P68" t="str">
+        <f>CONCATENATE(", ", M68, " ", N68, " ", O68)</f>
         <v>, CD_TYPE_ENG_NM VARCHAR2(100) NOT NULL</v>
       </c>
-      <c r="Q65" t="str">
-        <f t="shared" ref="Q65:Q74" si="11">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $M$64, ".", M65, " IS '", L65, "';")</f>
+      <c r="Q68" t="str">
+        <f t="shared" ref="Q68:Q77" si="15">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $M$67, ".", M68, " IS '", L68, "';")</f>
         <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CD_TYPE_ENG_NM IS '코드 분류 영문명';</v>
       </c>
-      <c r="R65" t="s">
-        <v>300</v>
-      </c>
-      <c r="V65" t="s">
+      <c r="R68" t="s">
+        <v>300</v>
+      </c>
+      <c r="V68" t="s">
         <v>22</v>
       </c>
-      <c r="W65" s="6" t="s">
+      <c r="W68" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="X65" s="6" t="s">
+      <c r="X68" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="Y65" s="6" t="s">
+      <c r="Y68" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Z65" s="6" t="s">
+      <c r="Z68" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="AA65" t="str">
-        <f>CONCATENATE(", ", X65, " ", Y65, " ", Z65)</f>
+      <c r="AA68" t="str">
+        <f>CONCATENATE(", ", X68, " ", Y68, " ", Z68)</f>
         <v>, ADM_CD VARCHAR2(100) NOT NULL</v>
       </c>
-      <c r="AB65" t="str">
-        <f t="shared" ref="AB65:AB71" si="12">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $X$64, ".", X65, " IS '", W65, "';")</f>
+      <c r="AB68" t="str">
+        <f t="shared" ref="AB68:AB74" si="16">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $X$67, ".", X68, " IS '", W68, "';")</f>
         <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.ADM_CD IS '관리자 코드';</v>
-      </c>
-    </row>
-    <row r="66" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>59</v>
-      </c>
-      <c r="D66" t="s">
-        <v>332</v>
-      </c>
-      <c r="E66" t="s">
-        <v>41</v>
-      </c>
-      <c r="G66" t="str">
-        <f t="shared" ref="G66:G77" si="13">CONCATENATE(", ", D66, " ", E66, " ", F66)</f>
-        <v xml:space="preserve">, USR_ID VARCHAR2(20) </v>
-      </c>
-      <c r="H66" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_ID IS '사용자 ID';</v>
-      </c>
-      <c r="I66" t="s">
-        <v>300</v>
-      </c>
-      <c r="L66" t="s">
-        <v>208</v>
-      </c>
-      <c r="M66" t="s">
-        <v>213</v>
-      </c>
-      <c r="N66" t="s">
-        <v>68</v>
-      </c>
-      <c r="P66" t="str">
-        <f t="shared" ref="P66:P74" si="14">CONCATENATE(", ", M66, " ", N66, " ", O66)</f>
-        <v xml:space="preserve">, CD_TYPE_ENG_ABRV_NM VARCHAR2(100) </v>
-      </c>
-      <c r="Q66" t="str">
-        <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CD_TYPE_ENG_ABRV_NM IS '코드 분류 영문 약어명';</v>
-      </c>
-      <c r="R66" t="s">
-        <v>300</v>
-      </c>
-      <c r="V66" t="s">
-        <v>22</v>
-      </c>
-      <c r="W66" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="X66" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="Y66" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z66" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="AA66" t="str">
-        <f t="shared" ref="AA66:AA71" si="15">CONCATENATE(", ", X66, " ", Y66, " ", Z66)</f>
-        <v>, USR_ID VARCHAR2(20) NOT NULL</v>
-      </c>
-      <c r="AB66" t="str">
-        <f t="shared" si="12"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.USR_ID IS '사용자 ID';</v>
-      </c>
-    </row>
-    <row r="67" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C67" t="s">
-        <v>67</v>
-      </c>
-      <c r="D67" t="s">
-        <v>74</v>
-      </c>
-      <c r="E67" t="s">
-        <v>68</v>
-      </c>
-      <c r="G67" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, USR_NM VARCHAR2(100) </v>
-      </c>
-      <c r="H67" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_NM IS '사용자 이름';</v>
-      </c>
-      <c r="I67" t="s">
-        <v>300</v>
-      </c>
-      <c r="L67" t="s">
-        <v>209</v>
-      </c>
-      <c r="M67" t="s">
-        <v>214</v>
-      </c>
-      <c r="N67" t="s">
-        <v>187</v>
-      </c>
-      <c r="P67" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">, CD_TYPE_KOR_NM VARCHAR2(200) </v>
-      </c>
-      <c r="Q67" t="str">
-        <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CD_TYPE_KOR_NM IS '코드 분류 한글명';</v>
-      </c>
-      <c r="R67" t="s">
-        <v>300</v>
-      </c>
-      <c r="W67" t="s">
-        <v>5</v>
-      </c>
-      <c r="X67" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y67" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z67" t="s">
-        <v>296</v>
-      </c>
-      <c r="AA67" t="str">
-        <f t="shared" si="15"/>
-        <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
-      </c>
-      <c r="AB67" t="str">
-        <f t="shared" si="12"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.DEL_YN IS '삭제 여부';</v>
-      </c>
-    </row>
-    <row r="68" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C68" t="s">
-        <v>64</v>
-      </c>
-      <c r="D68" t="s">
-        <v>133</v>
-      </c>
-      <c r="E68" t="s">
-        <v>41</v>
-      </c>
-      <c r="G68" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, USR_DEPT_ID VARCHAR2(20) </v>
-      </c>
-      <c r="H68" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_DEPT_ID IS '사용자 부서 ID';</v>
-      </c>
-      <c r="I68" t="s">
-        <v>300</v>
-      </c>
-      <c r="L68" t="s">
-        <v>210</v>
-      </c>
-      <c r="M68" t="s">
-        <v>214</v>
-      </c>
-      <c r="N68" t="s">
-        <v>54</v>
-      </c>
-      <c r="P68" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">, CD_TYPE_KOR_NM VARCHAR2(1000) </v>
-      </c>
-      <c r="Q68" t="str">
-        <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CD_TYPE_KOR_NM IS '코드 분류 설명';</v>
-      </c>
-      <c r="R68" t="s">
-        <v>300</v>
-      </c>
-      <c r="W68" t="s">
-        <v>15</v>
-      </c>
-      <c r="X68" t="s">
-        <v>289</v>
-      </c>
-      <c r="Y68" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z68" t="s">
-        <v>296</v>
-      </c>
-      <c r="AA68" t="str">
-        <f t="shared" si="15"/>
-        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
-      </c>
-      <c r="AB68" t="str">
-        <f t="shared" si="12"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.CRT_DT_TM IS '생성 일시';</v>
       </c>
     </row>
     <row r="69" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D69" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="E69" t="s">
+        <v>41</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" ref="G69:G80" si="17">CONCATENATE(", ", D69, " ", E69, " ", F69)</f>
+        <v xml:space="preserve">, USR_ID VARCHAR2(20) </v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_ID IS '사용자 ID';</v>
+      </c>
+      <c r="I69" t="s">
+        <v>300</v>
+      </c>
+      <c r="L69" t="s">
+        <v>208</v>
+      </c>
+      <c r="M69" t="s">
+        <v>213</v>
+      </c>
+      <c r="N69" t="s">
         <v>68</v>
       </c>
-      <c r="G69" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, USR_DEPT_NM VARCHAR2(100) </v>
-      </c>
-      <c r="H69" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_DEPT_NM IS '사용자 부서 명';</v>
-      </c>
-      <c r="I69" t="s">
-        <v>300</v>
-      </c>
-      <c r="L69" t="s">
-        <v>211</v>
-      </c>
-      <c r="M69" t="s">
-        <v>215</v>
-      </c>
-      <c r="N69" t="s">
-        <v>295</v>
-      </c>
       <c r="P69" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">, CD_TYPE_ORD INTEGER </v>
+        <f t="shared" ref="P69:P77" si="18">CONCATENATE(", ", M69, " ", N69, " ", O69)</f>
+        <v xml:space="preserve">, CD_TYPE_ENG_ABRV_NM VARCHAR2(100) </v>
       </c>
       <c r="Q69" t="str">
-        <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CD_TYPE_ORD IS '코드 분류 순서';</v>
+        <f t="shared" si="15"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CD_TYPE_ENG_ABRV_NM IS '코드 분류 영문 약어명';</v>
       </c>
       <c r="R69" t="s">
         <v>300</v>
       </c>
-      <c r="W69" t="s">
-        <v>6</v>
-      </c>
-      <c r="X69" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y69" t="s">
+      <c r="V69" t="s">
+        <v>22</v>
+      </c>
+      <c r="W69" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="X69" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="Y69" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Z69" t="s">
+      <c r="Z69" s="6" t="s">
         <v>296</v>
       </c>
       <c r="AA69" t="str">
-        <f t="shared" si="15"/>
-        <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
+        <f t="shared" ref="AA69:AA74" si="19">CONCATENATE(", ", X69, " ", Y69, " ", Z69)</f>
+        <v>, USR_ID VARCHAR2(20) NOT NULL</v>
       </c>
       <c r="AB69" t="str">
-        <f t="shared" si="12"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.CRT_USR_ID IS '생성자 ID';</v>
+        <f t="shared" si="16"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.USR_ID IS '사용자 ID';</v>
       </c>
     </row>
     <row r="70" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D70" t="s">
-        <v>340</v>
+        <v>74</v>
       </c>
       <c r="E70" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, USR_POS_ID VARCHAR2(20) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, USR_NM VARCHAR2(100) </v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_POS_ID IS '사용자 직위 ID';</v>
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_NM IS '사용자 이름';</v>
       </c>
       <c r="I70" t="s">
         <v>300</v>
       </c>
       <c r="L70" t="s">
+        <v>209</v>
+      </c>
+      <c r="M70" t="s">
+        <v>214</v>
+      </c>
+      <c r="N70" t="s">
+        <v>187</v>
+      </c>
+      <c r="P70" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, CD_TYPE_KOR_NM VARCHAR2(200) </v>
+      </c>
+      <c r="Q70" t="str">
+        <f t="shared" si="15"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CD_TYPE_KOR_NM IS '코드 분류 한글명';</v>
+      </c>
+      <c r="R70" t="s">
+        <v>300</v>
+      </c>
+      <c r="W70" t="s">
         <v>5</v>
       </c>
-      <c r="M70" t="s">
+      <c r="X70" t="s">
         <v>113</v>
       </c>
-      <c r="N70" t="s">
+      <c r="Y70" t="s">
         <v>40</v>
       </c>
-      <c r="O70" t="s">
+      <c r="Z70" t="s">
         <v>296</v>
       </c>
-      <c r="P70" t="str">
-        <f t="shared" si="14"/>
+      <c r="AA70" t="str">
+        <f t="shared" si="19"/>
         <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
       </c>
-      <c r="Q70" t="str">
-        <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.DEL_YN IS '삭제 여부';</v>
-      </c>
-      <c r="R70" t="s">
-        <v>300</v>
-      </c>
-      <c r="W70" t="s">
-        <v>16</v>
-      </c>
-      <c r="X70" t="s">
-        <v>302</v>
-      </c>
-      <c r="Y70" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA70" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
-      </c>
       <c r="AB70" t="str">
-        <f t="shared" si="12"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.MOD_DT_TM IS '수정 일시';</v>
+        <f t="shared" si="16"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.DEL_YN IS '삭제 여부';</v>
       </c>
     </row>
     <row r="71" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D71" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E71" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, USR_POS_NM VARCHAR2(100) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, USR_DEPT_ID VARCHAR2(20) </v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_POS_NM IS '사용자 직위 명';</v>
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_DEPT_ID IS '사용자 부서 ID';</v>
       </c>
       <c r="I71" t="s">
         <v>300</v>
       </c>
       <c r="L71" t="s">
+        <v>210</v>
+      </c>
+      <c r="M71" t="s">
+        <v>214</v>
+      </c>
+      <c r="N71" t="s">
+        <v>54</v>
+      </c>
+      <c r="P71" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, CD_TYPE_KOR_NM VARCHAR2(1000) </v>
+      </c>
+      <c r="Q71" t="str">
+        <f t="shared" si="15"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CD_TYPE_KOR_NM IS '코드 분류 설명';</v>
+      </c>
+      <c r="R71" t="s">
+        <v>300</v>
+      </c>
+      <c r="W71" t="s">
         <v>15</v>
       </c>
-      <c r="M71" t="s">
+      <c r="X71" t="s">
         <v>289</v>
       </c>
-      <c r="N71" t="s">
+      <c r="Y71" t="s">
         <v>43</v>
       </c>
-      <c r="O71" t="s">
+      <c r="Z71" t="s">
         <v>296</v>
       </c>
-      <c r="P71" t="str">
-        <f t="shared" si="14"/>
+      <c r="AA71" t="str">
+        <f t="shared" si="19"/>
         <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
       </c>
-      <c r="Q71" t="str">
-        <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CRT_DT_TM IS '생성 일시';</v>
-      </c>
-      <c r="R71" t="s">
-        <v>300</v>
-      </c>
-      <c r="W71" t="s">
-        <v>7</v>
-      </c>
-      <c r="X71" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y71" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA71" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">, MOD_USR_ID VARCHAR2(20) </v>
-      </c>
       <c r="AB71" t="str">
-        <f t="shared" si="12"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.MOD_USR_ID IS '수정자 ID';</v>
+        <f t="shared" si="16"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.CRT_DT_TM IS '생성 일시';</v>
       </c>
     </row>
     <row r="72" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>60</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>342</v>
+        <v>65</v>
+      </c>
+      <c r="D72" t="s">
+        <v>340</v>
       </c>
       <c r="E72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, USR_IP VARCHAR2(50) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, USR_DEPT_NM VARCHAR2(100) </v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_IP IS '사용자 IP';</v>
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_DEPT_NM IS '사용자 부서 명';</v>
       </c>
       <c r="I72" t="s">
         <v>300</v>
       </c>
       <c r="L72" t="s">
+        <v>211</v>
+      </c>
+      <c r="M72" t="s">
+        <v>215</v>
+      </c>
+      <c r="N72" t="s">
+        <v>295</v>
+      </c>
+      <c r="P72" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, CD_TYPE_ORD INTEGER </v>
+      </c>
+      <c r="Q72" t="str">
+        <f t="shared" si="15"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CD_TYPE_ORD IS '코드 분류 순서';</v>
+      </c>
+      <c r="R72" t="s">
+        <v>300</v>
+      </c>
+      <c r="W72" t="s">
         <v>6</v>
       </c>
-      <c r="M72" t="s">
+      <c r="X72" t="s">
         <v>75</v>
       </c>
-      <c r="N72" t="s">
+      <c r="Y72" t="s">
         <v>41</v>
       </c>
-      <c r="O72" t="s">
+      <c r="Z72" t="s">
         <v>296</v>
       </c>
-      <c r="P72" t="str">
-        <f t="shared" si="14"/>
+      <c r="AA72" t="str">
+        <f t="shared" si="19"/>
         <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
       </c>
-      <c r="Q72" t="str">
-        <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CRT_USR_ID IS '생성자 ID';</v>
-      </c>
-      <c r="R72" t="s">
-        <v>300</v>
+      <c r="AB72" t="str">
+        <f t="shared" si="16"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.CRT_USR_ID IS '생성자 ID';</v>
       </c>
     </row>
     <row r="73" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>278</v>
+        <v>339</v>
       </c>
       <c r="E73" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, SCRN_ID VARCHAR2(100) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, USR_POS_ID VARCHAR2(20) </v>
       </c>
       <c r="H73" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.SCRN_ID IS '화면 ID';</v>
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_POS_ID IS '사용자 직위 ID';</v>
       </c>
       <c r="I73" t="s">
         <v>300</v>
       </c>
       <c r="L73" t="s">
+        <v>5</v>
+      </c>
+      <c r="M73" t="s">
+        <v>113</v>
+      </c>
+      <c r="N73" t="s">
+        <v>40</v>
+      </c>
+      <c r="O73" t="s">
+        <v>296</v>
+      </c>
+      <c r="P73" t="str">
+        <f t="shared" si="18"/>
+        <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
+      </c>
+      <c r="Q73" t="str">
+        <f t="shared" si="15"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.DEL_YN IS '삭제 여부';</v>
+      </c>
+      <c r="R73" t="s">
+        <v>300</v>
+      </c>
+      <c r="W73" t="s">
         <v>16</v>
       </c>
-      <c r="M73" t="s">
+      <c r="X73" t="s">
         <v>302</v>
       </c>
-      <c r="N73" t="s">
+      <c r="Y73" t="s">
         <v>43</v>
       </c>
-      <c r="P73" t="str">
-        <f t="shared" si="14"/>
+      <c r="AA73" t="str">
+        <f t="shared" si="19"/>
         <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
       </c>
-      <c r="Q73" t="str">
-        <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.MOD_DT_TM IS '수정 일시';</v>
-      </c>
-      <c r="R73" t="s">
-        <v>300</v>
+      <c r="AB73" t="str">
+        <f t="shared" si="16"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.MOD_DT_TM IS '수정 일시';</v>
       </c>
     </row>
     <row r="74" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D74" t="s">
-        <v>343</v>
+        <v>137</v>
       </c>
       <c r="E74" t="s">
         <v>68</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, SCRN_DET_ID VARCHAR2(100) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, USR_POS_NM VARCHAR2(100) </v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.SCRN_DET_ID IS '화면 상세 ID';</v>
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_POS_NM IS '사용자 직위 명';</v>
       </c>
       <c r="I74" t="s">
         <v>300</v>
       </c>
       <c r="L74" t="s">
+        <v>15</v>
+      </c>
+      <c r="M74" t="s">
+        <v>289</v>
+      </c>
+      <c r="N74" t="s">
+        <v>43</v>
+      </c>
+      <c r="O74" t="s">
+        <v>296</v>
+      </c>
+      <c r="P74" t="str">
+        <f t="shared" si="18"/>
+        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
+      </c>
+      <c r="Q74" t="str">
+        <f t="shared" si="15"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CRT_DT_TM IS '생성 일시';</v>
+      </c>
+      <c r="R74" t="s">
+        <v>300</v>
+      </c>
+      <c r="W74" t="s">
         <v>7</v>
       </c>
-      <c r="M74" t="s">
+      <c r="X74" t="s">
         <v>118</v>
       </c>
-      <c r="N74" t="s">
+      <c r="Y74" t="s">
         <v>41</v>
       </c>
-      <c r="P74" t="str">
-        <f t="shared" si="14"/>
+      <c r="AA74" t="str">
+        <f t="shared" si="19"/>
         <v xml:space="preserve">, MOD_USR_ID VARCHAR2(20) </v>
       </c>
-      <c r="Q74" t="str">
-        <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.MOD_USR_ID IS '수정자 ID';</v>
-      </c>
-      <c r="R74" t="s">
-        <v>300</v>
+      <c r="AB74" t="str">
+        <f t="shared" si="16"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_ADMIN.MOD_USR_ID IS '수정자 ID';</v>
       </c>
     </row>
     <row r="75" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
-        <v>63</v>
-      </c>
-      <c r="D75" t="s">
-        <v>344</v>
+        <v>60</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>341</v>
       </c>
       <c r="E75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, USR_ACTN VARCHAR2(20) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, USR_IP VARCHAR2(50) </v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_ACTN IS '사용자 행동';</v>
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_IP IS '사용자 IP';</v>
       </c>
       <c r="I75" t="s">
         <v>300</v>
       </c>
-      <c r="W75" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="X75" t="s">
-        <v>359</v>
+      <c r="L75" t="s">
+        <v>6</v>
+      </c>
+      <c r="M75" t="s">
+        <v>75</v>
+      </c>
+      <c r="N75" t="s">
+        <v>41</v>
+      </c>
+      <c r="O75" t="s">
+        <v>296</v>
+      </c>
+      <c r="P75" t="str">
+        <f t="shared" si="18"/>
+        <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
+      </c>
+      <c r="Q75" t="str">
+        <f t="shared" si="15"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.CRT_USR_ID IS '생성자 ID';</v>
+      </c>
+      <c r="R75" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="76" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D76" t="s">
-        <v>150</v>
+        <v>278</v>
       </c>
       <c r="E76" t="s">
-        <v>301</v>
+        <v>68</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">, DET_INFO_MAP VARCHAR2(2000) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, SCRN_ID VARCHAR2(100) </v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.DET_INFO_MAP IS '상세 정보';</v>
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.SCRN_ID IS '화면 ID';</v>
       </c>
       <c r="I76" t="s">
         <v>300</v>
       </c>
-      <c r="V76" t="s">
-        <v>22</v>
-      </c>
-      <c r="W76" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="X76" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="Y76" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="Z76" s="6" t="s">
-        <v>296</v>
+      <c r="L76" t="s">
+        <v>16</v>
+      </c>
+      <c r="M76" t="s">
+        <v>302</v>
+      </c>
+      <c r="N76" t="s">
+        <v>43</v>
+      </c>
+      <c r="P76" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
+      </c>
+      <c r="Q76" t="str">
+        <f t="shared" si="15"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.MOD_DT_TM IS '수정 일시';</v>
+      </c>
+      <c r="R76" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="77" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
+        <v>62</v>
+      </c>
+      <c r="D77" t="s">
+        <v>342</v>
+      </c>
+      <c r="E77" t="s">
+        <v>68</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, SCRN_DET_ID VARCHAR2(100) </v>
+      </c>
+      <c r="H77" t="str">
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.SCRN_DET_ID IS '화면 상세 ID';</v>
+      </c>
+      <c r="I77" t="s">
+        <v>300</v>
+      </c>
+      <c r="L77" t="s">
+        <v>7</v>
+      </c>
+      <c r="M77" t="s">
+        <v>118</v>
+      </c>
+      <c r="N77" t="s">
+        <v>41</v>
+      </c>
+      <c r="P77" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, MOD_USR_ID VARCHAR2(20) </v>
+      </c>
+      <c r="Q77" t="str">
+        <f t="shared" si="15"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE_TYPE.MOD_USR_ID IS '수정자 ID';</v>
+      </c>
+      <c r="R77" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="78" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>63</v>
+      </c>
+      <c r="D78" t="s">
+        <v>343</v>
+      </c>
+      <c r="E78" t="s">
+        <v>70</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, USR_ACTN VARCHAR2(20) </v>
+      </c>
+      <c r="H78" t="str">
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.USR_ACTN IS '사용자 행동';</v>
+      </c>
+      <c r="I78" t="s">
+        <v>300</v>
+      </c>
+      <c r="W78" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X78" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="79" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>66</v>
+      </c>
+      <c r="D79" t="s">
+        <v>150</v>
+      </c>
+      <c r="E79" t="s">
+        <v>301</v>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">, DET_INFO_MAP VARCHAR2(2000) </v>
+      </c>
+      <c r="H79" t="str">
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.DET_INFO_MAP IS '상세 정보';</v>
+      </c>
+      <c r="I79" t="s">
+        <v>300</v>
+      </c>
+      <c r="V79" t="s">
+        <v>22</v>
+      </c>
+      <c r="W79" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="X79" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y79" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="Z79" s="6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="80" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
         <v>15</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D80" t="s">
         <v>289</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E80" t="s">
         <v>43</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F80" t="s">
         <v>296</v>
       </c>
-      <c r="G77" t="str">
-        <f t="shared" si="13"/>
-        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
-      </c>
-      <c r="H77" t="str">
-        <f t="shared" si="10"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.CRT_DT_TM IS '생성 일시';</v>
-      </c>
-      <c r="I77" t="s">
-        <v>300</v>
-      </c>
-      <c r="W77" t="s">
-        <v>269</v>
-      </c>
-      <c r="X77" t="s">
-        <v>270</v>
-      </c>
-      <c r="Y77" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="78" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="L78" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="M78" t="s">
-        <v>358</v>
-      </c>
-      <c r="Q78" t="str">
-        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $M$78, " IS '", L78, "';")</f>
-        <v>COMMENT ON TABLE PORTAL.PT_PORTAL_CODE IS '포탈 코드 테이블';</v>
-      </c>
-      <c r="R78" t="s">
-        <v>300</v>
-      </c>
-      <c r="W78" t="s">
-        <v>271</v>
-      </c>
-      <c r="X78" t="s">
-        <v>272</v>
-      </c>
-      <c r="Y78" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="79" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="K79" t="s">
-        <v>22</v>
-      </c>
-      <c r="L79" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="M79" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="N79" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O79" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="P79" t="str">
-        <f>CONCATENATE(", ", M79, " ", N79, " ", O79)</f>
-        <v>, CD_TYPE_ENG_NM VARCHAR2(100) NOT NULL</v>
-      </c>
-      <c r="Q79" t="str">
-        <f t="shared" ref="Q79:Q89" si="16">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $M$78, ".", M79, " IS '", L79, "';")</f>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_TYPE_ENG_NM IS '코드 분류 영문명';</v>
-      </c>
-      <c r="R79" t="s">
-        <v>300</v>
-      </c>
-      <c r="W79" t="s">
-        <v>284</v>
-      </c>
-      <c r="X79" t="s">
-        <v>285</v>
-      </c>
-      <c r="Y79" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="80" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="K80" t="s">
-        <v>22</v>
-      </c>
-      <c r="L80" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="M80" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="N80" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O80" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="P80" t="str">
-        <f t="shared" ref="P80:P89" si="17">CONCATENATE(", ", M80, " ", N80, " ", O80)</f>
-        <v>, CD_ENG_NM VARCHAR2(100) NOT NULL</v>
-      </c>
-      <c r="Q80" t="str">
-        <f t="shared" si="16"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_ENG_NM IS '코드 영문명';</v>
-      </c>
-      <c r="R80" t="s">
-        <v>300</v>
-      </c>
-      <c r="W80" t="s">
-        <v>267</v>
-      </c>
-      <c r="X80" t="s">
-        <v>273</v>
-      </c>
-      <c r="Y80" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="81" spans="12:26" x14ac:dyDescent="0.3">
-      <c r="L81" t="s">
-        <v>166</v>
-      </c>
-      <c r="M81" t="s">
-        <v>186</v>
-      </c>
-      <c r="N81" t="s">
-        <v>68</v>
-      </c>
-      <c r="P81" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">, CD_ENG_ABRV_NM VARCHAR2(100) </v>
-      </c>
-      <c r="Q81" t="str">
-        <f t="shared" si="16"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_ENG_ABRV_NM IS '코드 영문 약어명';</v>
-      </c>
-      <c r="R81" t="s">
-        <v>300</v>
-      </c>
-      <c r="W81" t="s">
-        <v>274</v>
-      </c>
-      <c r="X81" t="s">
-        <v>275</v>
-      </c>
-      <c r="Y81" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="82" spans="12:26" x14ac:dyDescent="0.3">
-      <c r="L82" t="s">
-        <v>167</v>
-      </c>
-      <c r="M82" t="s">
-        <v>182</v>
-      </c>
-      <c r="N82" t="s">
-        <v>187</v>
-      </c>
-      <c r="P82" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">, CD_KOR_NM VARCHAR2(200) </v>
-      </c>
-      <c r="Q82" t="str">
-        <f t="shared" si="16"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_KOR_NM IS '코드 한글명';</v>
-      </c>
-      <c r="R82" t="s">
-        <v>300</v>
-      </c>
-      <c r="W82" t="s">
-        <v>277</v>
-      </c>
-      <c r="X82" t="s">
-        <v>276</v>
-      </c>
-      <c r="Y82" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="83" spans="12:26" x14ac:dyDescent="0.3">
-      <c r="L83" t="s">
-        <v>168</v>
-      </c>
-      <c r="M83" t="s">
-        <v>182</v>
-      </c>
-      <c r="N83" t="s">
-        <v>54</v>
-      </c>
-      <c r="P83" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">, CD_KOR_NM VARCHAR2(1000) </v>
-      </c>
-      <c r="Q83" t="str">
-        <f t="shared" si="16"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_KOR_NM IS '코드 설명';</v>
-      </c>
-      <c r="R83" t="s">
-        <v>300</v>
-      </c>
-      <c r="W83" t="s">
-        <v>265</v>
-      </c>
-      <c r="X83" t="s">
-        <v>279</v>
-      </c>
-      <c r="Y83" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="84" spans="12:26" x14ac:dyDescent="0.3">
-      <c r="L84" t="s">
-        <v>189</v>
-      </c>
-      <c r="M84" t="s">
-        <v>193</v>
-      </c>
-      <c r="N84" t="s">
-        <v>295</v>
-      </c>
-      <c r="P84" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">, CD_ORD INTEGER </v>
-      </c>
-      <c r="Q84" t="str">
-        <f t="shared" si="16"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_ORD IS '코드 순서';</v>
-      </c>
-      <c r="R84" t="s">
-        <v>300</v>
-      </c>
-      <c r="W84" t="s">
-        <v>266</v>
-      </c>
-      <c r="X84" t="s">
-        <v>283</v>
-      </c>
-      <c r="Y84" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="85" spans="12:26" x14ac:dyDescent="0.3">
-      <c r="L85" t="s">
-        <v>5</v>
-      </c>
-      <c r="M85" t="s">
-        <v>113</v>
-      </c>
-      <c r="N85" t="s">
-        <v>40</v>
-      </c>
-      <c r="O85" t="s">
-        <v>296</v>
-      </c>
-      <c r="P85" t="str">
-        <f t="shared" si="17"/>
-        <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
-      </c>
-      <c r="Q85" t="str">
-        <f t="shared" si="16"/>
-        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.DEL_YN IS '삭제 여부';</v>
-      </c>
-      <c r="R85" t="s">
-        <v>300</v>
-      </c>
-      <c r="W85" t="s">
-        <v>5</v>
-      </c>
-      <c r="X85" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y85" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z85" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="86" spans="12:26" x14ac:dyDescent="0.3">
-      <c r="L86" t="s">
-        <v>15</v>
-      </c>
-      <c r="M86" t="s">
-        <v>289</v>
-      </c>
-      <c r="N86" t="s">
-        <v>43</v>
-      </c>
-      <c r="O86" t="s">
-        <v>296</v>
-      </c>
-      <c r="P86" t="str">
+      <c r="G80" t="str">
         <f t="shared" si="17"/>
         <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
       </c>
+      <c r="H80" t="str">
+        <f t="shared" si="14"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_LOG.CRT_DT_TM IS '생성 일시';</v>
+      </c>
+      <c r="I80" t="s">
+        <v>300</v>
+      </c>
+      <c r="W80" t="s">
+        <v>269</v>
+      </c>
+      <c r="X80" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="81" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L81" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="M81" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q81" t="str">
+        <f>CONCATENATE("COMMENT ON TABLE ", $A$1, ".", $M$81, " IS '", L81, "';")</f>
+        <v>COMMENT ON TABLE PORTAL.PT_PORTAL_CODE IS '포탈 코드 테이블';</v>
+      </c>
+      <c r="R81" t="s">
+        <v>300</v>
+      </c>
+      <c r="W81" t="s">
+        <v>271</v>
+      </c>
+      <c r="X81" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="K82" t="s">
+        <v>22</v>
+      </c>
+      <c r="L82" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="M82" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="N82" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="O82" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="P82" t="str">
+        <f>CONCATENATE(", ", M82, " ", N82, " ", O82)</f>
+        <v>, CD_TYPE_ENG_NM VARCHAR2(100) NOT NULL</v>
+      </c>
+      <c r="Q82" t="str">
+        <f t="shared" ref="Q82:Q92" si="20">CONCATENATE("COMMENT ON COLUMN ", $A$1, ".", $M$81, ".", M82, " IS '", L82, "';")</f>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_TYPE_ENG_NM IS '코드 분류 영문명';</v>
+      </c>
+      <c r="R82" t="s">
+        <v>300</v>
+      </c>
+      <c r="W82" t="s">
+        <v>284</v>
+      </c>
+      <c r="X82" t="s">
+        <v>285</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="83" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="K83" t="s">
+        <v>22</v>
+      </c>
+      <c r="L83" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="M83" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="N83" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="O83" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="P83" t="str">
+        <f t="shared" ref="P83:P92" si="21">CONCATENATE(", ", M83, " ", N83, " ", O83)</f>
+        <v>, CD_ENG_NM VARCHAR2(100) NOT NULL</v>
+      </c>
+      <c r="Q83" t="str">
+        <f t="shared" si="20"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_ENG_NM IS '코드 영문명';</v>
+      </c>
+      <c r="R83" t="s">
+        <v>300</v>
+      </c>
+      <c r="W83" t="s">
+        <v>267</v>
+      </c>
+      <c r="X83" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="84" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L84" t="s">
+        <v>166</v>
+      </c>
+      <c r="M84" t="s">
+        <v>186</v>
+      </c>
+      <c r="N84" t="s">
+        <v>68</v>
+      </c>
+      <c r="P84" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">, CD_ENG_ABRV_NM VARCHAR2(100) </v>
+      </c>
+      <c r="Q84" t="str">
+        <f t="shared" si="20"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_ENG_ABRV_NM IS '코드 영문 약어명';</v>
+      </c>
+      <c r="R84" t="s">
+        <v>300</v>
+      </c>
+      <c r="W84" t="s">
+        <v>274</v>
+      </c>
+      <c r="X84" t="s">
+        <v>275</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="85" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L85" t="s">
+        <v>167</v>
+      </c>
+      <c r="M85" t="s">
+        <v>182</v>
+      </c>
+      <c r="N85" t="s">
+        <v>187</v>
+      </c>
+      <c r="P85" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">, CD_KOR_NM VARCHAR2(200) </v>
+      </c>
+      <c r="Q85" t="str">
+        <f t="shared" si="20"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_KOR_NM IS '코드 한글명';</v>
+      </c>
+      <c r="R85" t="s">
+        <v>300</v>
+      </c>
+      <c r="W85" t="s">
+        <v>277</v>
+      </c>
+      <c r="X85" t="s">
+        <v>276</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="86" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L86" t="s">
+        <v>168</v>
+      </c>
+      <c r="M86" t="s">
+        <v>182</v>
+      </c>
+      <c r="N86" t="s">
+        <v>54</v>
+      </c>
+      <c r="P86" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">, CD_KOR_NM VARCHAR2(1000) </v>
+      </c>
       <c r="Q86" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_KOR_NM IS '코드 설명';</v>
+      </c>
+      <c r="R86" t="s">
+        <v>300</v>
+      </c>
+      <c r="W86" t="s">
+        <v>265</v>
+      </c>
+      <c r="X86" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="87" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L87" t="s">
+        <v>189</v>
+      </c>
+      <c r="M87" t="s">
+        <v>193</v>
+      </c>
+      <c r="N87" t="s">
+        <v>295</v>
+      </c>
+      <c r="P87" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">, CD_ORD INTEGER </v>
+      </c>
+      <c r="Q87" t="str">
+        <f t="shared" si="20"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CD_ORD IS '코드 순서';</v>
+      </c>
+      <c r="R87" t="s">
+        <v>300</v>
+      </c>
+      <c r="W87" t="s">
+        <v>266</v>
+      </c>
+      <c r="X87" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="88" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L88" t="s">
+        <v>5</v>
+      </c>
+      <c r="M88" t="s">
+        <v>113</v>
+      </c>
+      <c r="N88" t="s">
+        <v>40</v>
+      </c>
+      <c r="O88" t="s">
+        <v>296</v>
+      </c>
+      <c r="P88" t="str">
+        <f t="shared" si="21"/>
+        <v>, DEL_YN VARCHAR2(1) NOT NULL</v>
+      </c>
+      <c r="Q88" t="str">
+        <f t="shared" si="20"/>
+        <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.DEL_YN IS '삭제 여부';</v>
+      </c>
+      <c r="R88" t="s">
+        <v>300</v>
+      </c>
+      <c r="W88" t="s">
+        <v>5</v>
+      </c>
+      <c r="X88" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y88" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z88" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="89" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L89" t="s">
+        <v>15</v>
+      </c>
+      <c r="M89" t="s">
+        <v>289</v>
+      </c>
+      <c r="N89" t="s">
+        <v>43</v>
+      </c>
+      <c r="O89" t="s">
+        <v>296</v>
+      </c>
+      <c r="P89" t="str">
+        <f t="shared" si="21"/>
+        <v>, CRT_DT_TM TIMESTAMP NOT NULL</v>
+      </c>
+      <c r="Q89" t="str">
+        <f t="shared" si="20"/>
         <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CRT_DT_TM IS '생성 일시';</v>
       </c>
-      <c r="R86" t="s">
-        <v>300</v>
-      </c>
-      <c r="W86" t="s">
+      <c r="R89" t="s">
+        <v>300</v>
+      </c>
+      <c r="W89" t="s">
         <v>15</v>
       </c>
-      <c r="X86" t="s">
+      <c r="X89" t="s">
         <v>289</v>
       </c>
-      <c r="Y86" t="s">
+      <c r="Y89" t="s">
         <v>43</v>
       </c>
-      <c r="Z86" t="s">
+      <c r="Z89" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="87" spans="12:26" x14ac:dyDescent="0.3">
-      <c r="L87" t="s">
+    <row r="90" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L90" t="s">
         <v>6</v>
       </c>
-      <c r="M87" t="s">
+      <c r="M90" t="s">
         <v>75</v>
       </c>
-      <c r="N87" t="s">
+      <c r="N90" t="s">
         <v>41</v>
       </c>
-      <c r="O87" t="s">
+      <c r="O90" t="s">
         <v>296</v>
       </c>
-      <c r="P87" t="str">
-        <f t="shared" si="17"/>
+      <c r="P90" t="str">
+        <f t="shared" si="21"/>
         <v>, CRT_USR_ID VARCHAR2(20) NOT NULL</v>
       </c>
-      <c r="Q87" t="str">
-        <f t="shared" si="16"/>
+      <c r="Q90" t="str">
+        <f t="shared" si="20"/>
         <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.CRT_USR_ID IS '생성자 ID';</v>
       </c>
-      <c r="R87" t="s">
-        <v>300</v>
-      </c>
-      <c r="W87" t="s">
+      <c r="R90" t="s">
+        <v>300</v>
+      </c>
+      <c r="W90" t="s">
         <v>6</v>
       </c>
-      <c r="X87" t="s">
+      <c r="X90" t="s">
         <v>75</v>
       </c>
-      <c r="Y87" t="s">
+      <c r="Y90" t="s">
         <v>41</v>
       </c>
-      <c r="Z87" t="s">
+      <c r="Z90" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="88" spans="12:26" x14ac:dyDescent="0.3">
-      <c r="L88" t="s">
+    <row r="91" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L91" t="s">
         <v>16</v>
       </c>
-      <c r="M88" t="s">
+      <c r="M91" t="s">
         <v>302</v>
       </c>
-      <c r="N88" t="s">
+      <c r="N91" t="s">
         <v>43</v>
       </c>
-      <c r="P88" t="str">
-        <f t="shared" si="17"/>
+      <c r="P91" t="str">
+        <f t="shared" si="21"/>
         <v xml:space="preserve">, MOD_DT_TM TIMESTAMP </v>
       </c>
-      <c r="Q88" t="str">
-        <f t="shared" si="16"/>
+      <c r="Q91" t="str">
+        <f t="shared" si="20"/>
         <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.MOD_DT_TM IS '수정 일시';</v>
       </c>
-      <c r="R88" t="s">
-        <v>300</v>
-      </c>
-      <c r="W88" t="s">
+      <c r="R91" t="s">
+        <v>300</v>
+      </c>
+      <c r="W91" t="s">
         <v>16</v>
       </c>
-      <c r="X88" t="s">
+      <c r="X91" t="s">
         <v>302</v>
       </c>
-      <c r="Y88" t="s">
+      <c r="Y91" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="12:26" x14ac:dyDescent="0.3">
-      <c r="L89" t="s">
+    <row r="92" spans="11:26" x14ac:dyDescent="0.3">
+      <c r="L92" t="s">
         <v>7</v>
       </c>
-      <c r="M89" t="s">
+      <c r="M92" t="s">
         <v>118</v>
       </c>
-      <c r="N89" t="s">
+      <c r="N92" t="s">
         <v>41</v>
       </c>
-      <c r="P89" t="str">
-        <f t="shared" si="17"/>
+      <c r="P92" t="str">
+        <f t="shared" si="21"/>
         <v xml:space="preserve">, MOD_USR_ID VARCHAR2(20) </v>
       </c>
-      <c r="Q89" t="str">
-        <f t="shared" si="16"/>
+      <c r="Q92" t="str">
+        <f t="shared" si="20"/>
         <v>COMMENT ON COLUMN PORTAL.PT_PORTAL_CODE.MOD_USR_ID IS '수정자 ID';</v>
       </c>
-      <c r="R89" t="s">
-        <v>300</v>
-      </c>
-      <c r="W89" t="s">
+      <c r="R92" t="s">
+        <v>300</v>
+      </c>
+      <c r="W92" t="s">
         <v>7</v>
       </c>
-      <c r="X89" t="s">
+      <c r="X92" t="s">
         <v>118</v>
       </c>
-      <c r="Y89" t="s">
+      <c r="Y92" t="s">
         <v>41</v>
       </c>
     </row>
@@ -6608,10 +6728,10 @@
         <v>230</v>
       </c>
       <c r="D4" t="s">
+        <v>345</v>
+      </c>
+      <c r="F4" t="s">
         <v>346</v>
-      </c>
-      <c r="F4" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -6650,10 +6770,10 @@
         <v>237</v>
       </c>
       <c r="D7" t="s">
+        <v>347</v>
+      </c>
+      <c r="F7" t="s">
         <v>348</v>
-      </c>
-      <c r="F7" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -6664,7 +6784,7 @@
         <v>237</v>
       </c>
       <c r="D8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F8" t="s">
         <v>254</v>
@@ -6706,7 +6826,7 @@
         <v>239</v>
       </c>
       <c r="D11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F11" t="s">
         <v>240</v>
@@ -6720,7 +6840,7 @@
         <v>239</v>
       </c>
       <c r="D12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F12" t="s">
         <v>243</v>
@@ -6802,20 +6922,20 @@
         <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C3" t="s">
         <v>334</v>
-      </c>
-      <c r="C3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -6845,7 +6965,7 @@
         <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
@@ -6855,12 +6975,12 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="G7" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="11"/>
@@ -6872,7 +6992,7 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="G8" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8" t="s">
@@ -6880,7 +7000,7 @@
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="8" t="s">
@@ -6890,11 +7010,11 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="G9" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="11"/>
@@ -6904,15 +7024,15 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="G10" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="11"/>
@@ -6920,7 +7040,7 @@
     </row>
     <row r="11" spans="2:14" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="11"/>
@@ -6932,7 +7052,7 @@
     </row>
     <row r="12" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G12" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="11"/>

</xml_diff>